<commit_message>
fix random joint issue
</commit_message>
<xml_diff>
--- a/notebooks/simulation/sim_results/summary_norm_dist_000_test.xlsx
+++ b/notebooks/simulation/sim_results/summary_norm_dist_000_test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,64 +568,64 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3635795477609886</v>
+        <v>0.7271590955219772</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2262208220942797</v>
+        <v>0.4524416441885594</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4654304383294138</v>
+        <v>0.9308608766588276</v>
       </c>
       <c r="H2" t="n">
-        <v>0.387016467396819</v>
+        <v>0.774032934793638</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2464179588392459</v>
+        <v>0.4928359176784918</v>
       </c>
       <c r="K2" t="n">
-        <v>0.3837114193728477</v>
+        <v>0.7674228387456954</v>
       </c>
       <c r="L2" t="n">
-        <v>0.4153847705612123</v>
+        <v>0.8307695411224246</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>0.3702993539951823</v>
+        <v>0.7405987079903645</v>
       </c>
       <c r="O2" t="n">
-        <v>0.4348233892816828</v>
+        <v>0.8696467785633657</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4226654411933767</v>
+        <v>0.8425683631632674</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.4168887731400137</v>
+        <v>0.8337775462800274</v>
       </c>
       <c r="R2" t="n">
-        <v>0.3975497447594747</v>
+        <v>0.7950994895189494</v>
       </c>
       <c r="S2" t="n">
-        <v>0.4410864989152133</v>
+        <v>0.8821729978304266</v>
       </c>
       <c r="T2" t="n">
-        <v>0.3588831080905508</v>
+        <v>0.7177662161811016</v>
       </c>
       <c r="U2" t="n">
-        <v>0.1587434782643155</v>
+        <v>0.317486956528631</v>
       </c>
       <c r="V2" t="n">
-        <v>0.4704083702492194</v>
+        <v>0.9408167404984388</v>
       </c>
       <c r="W2" t="n">
-        <v>0.4787982194341486</v>
+        <v>0.9575964388682972</v>
       </c>
       <c r="X2" t="n">
-        <v>0.465135379766708</v>
+        <v>0.930270759533416</v>
       </c>
     </row>
     <row r="3">
@@ -646,64 +646,64 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2928674415204748</v>
+        <v>0.5857348830409497</v>
       </c>
       <c r="F3" t="n">
-        <v>0.01627198286981698</v>
+        <v>0.03254396573963395</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2153474565900104</v>
+        <v>0.4306949131800209</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4163303179826275</v>
+        <v>0.8326606359652551</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00154462542434855</v>
+        <v>0.0030892508486971</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4344071456163237</v>
+        <v>0.8688142912326473</v>
       </c>
       <c r="L3" t="n">
-        <v>0.419882283769351</v>
+        <v>0.839764567538702</v>
       </c>
       <c r="M3" t="n">
-        <v>0.4826458531089068</v>
+        <v>0.643527804145209</v>
       </c>
       <c r="N3" t="n">
-        <v>0.4241876654410827</v>
+        <v>0.8483753308821654</v>
       </c>
       <c r="O3" t="n">
-        <v>0.4071912476770889</v>
+        <v>0.8143824953541777</v>
       </c>
       <c r="P3" t="n">
-        <v>0.4159312581620858</v>
+        <v>0.8291440113688637</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.3805746637252123</v>
+        <v>0.7611493274504246</v>
       </c>
       <c r="R3" t="n">
-        <v>0.2482035503032128</v>
+        <v>0.4964071006064256</v>
       </c>
       <c r="S3" t="n">
-        <v>0.3779718296614912</v>
+        <v>0.7559436593229824</v>
       </c>
       <c r="T3" t="n">
-        <v>0.0385783462684233</v>
+        <v>0.07715669253684659</v>
       </c>
       <c r="U3" t="n">
-        <v>0.2603532816251828</v>
+        <v>0.5207065632503656</v>
       </c>
       <c r="V3" t="n">
-        <v>0.4653058340085984</v>
+        <v>0.9306116680171967</v>
       </c>
       <c r="W3" t="n">
-        <v>0.4360377900166131</v>
+        <v>0.8720755800332262</v>
       </c>
       <c r="X3" t="n">
-        <v>0.4537990532059044</v>
+        <v>0.9075981064118088</v>
       </c>
     </row>
     <row r="4">
@@ -724,64 +724,64 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3296864087393601</v>
+        <v>0.6593728174787202</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2267185793449648</v>
+        <v>0.4534371586899295</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4627243506777312</v>
+        <v>0.9254487013554624</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3582582368587357</v>
+        <v>0.7165164737174714</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2369647893924725</v>
+        <v>0.4739295787849449</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4216043512535194</v>
+        <v>0.8432087025070387</v>
       </c>
       <c r="L4" t="n">
-        <v>0.3369432158559855</v>
+        <v>0.6738864317119709</v>
       </c>
       <c r="M4" t="n">
-        <v>0.02182935689984113</v>
+        <v>0.02910580919978817</v>
       </c>
       <c r="N4" t="n">
-        <v>0.3241054336984608</v>
+        <v>0.6482108673969216</v>
       </c>
       <c r="O4" t="n">
-        <v>0.3827133639401794</v>
+        <v>0.7654267278803587</v>
       </c>
       <c r="P4" t="n">
-        <v>0.4103667084264151</v>
+        <v>0.818051281503638</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.397421445434827</v>
+        <v>0.7948428908696541</v>
       </c>
       <c r="R4" t="n">
-        <v>0.280015323792033</v>
+        <v>0.560030647584066</v>
       </c>
       <c r="S4" t="n">
-        <v>0.4659627912400983</v>
+        <v>0.9319255824801966</v>
       </c>
       <c r="T4" t="n">
-        <v>0.3248102126936359</v>
+        <v>0.6496204253872718</v>
       </c>
       <c r="U4" t="n">
-        <v>0.179353838761476</v>
+        <v>0.3587076775229521</v>
       </c>
       <c r="V4" t="n">
-        <v>0.4656123089511354</v>
+        <v>0.9312246179022708</v>
       </c>
       <c r="W4" t="n">
-        <v>0.3829762300855307</v>
+        <v>0.7659524601710614</v>
       </c>
       <c r="X4" t="n">
-        <v>0.4586184047186697</v>
+        <v>0.9172368094373394</v>
       </c>
     </row>
     <row r="5">
@@ -790,76 +790,76 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>flowbot</t>
+          <t>hisditonly</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>sgp</t>
+          <t>raw</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3569139279798322</v>
+        <v>0.4018885160030032</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4644855536375428</v>
+        <v>0.3999951530291327</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4757230054366046</v>
+        <v>0.2588553441903752</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4759317164378512</v>
+        <v>0.956465370369235</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4685104960498358</v>
+        <v>0.4552275937912256</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4621222998892404</v>
+        <v>0.9423531717800028</v>
       </c>
       <c r="L5" t="n">
-        <v>0.4294681755092934</v>
+        <v>0.6167866004919149</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2311753752567467</v>
+        <v>0.6377611821860422</v>
       </c>
       <c r="N5" t="n">
-        <v>0.466829079307084</v>
+        <v>0.7888863170440094</v>
       </c>
       <c r="O5" t="n">
-        <v>0.4757043077308692</v>
+        <v>0.8775635475843448</v>
       </c>
       <c r="P5" t="n">
-        <v>0.4489028652738315</v>
+        <v>0.7874312500872318</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.425913110712731</v>
+        <v>0.7353826711300609</v>
       </c>
       <c r="R5" t="n">
-        <v>0.4631988399137653</v>
+        <v>0.5349590702337547</v>
       </c>
       <c r="S5" t="n">
-        <v>0.4574878114561474</v>
+        <v>0.7192495607071194</v>
       </c>
       <c r="T5" t="n">
-        <v>0.4628870996828708</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>0.1578734317553248</v>
+        <v>0.3168898335349684</v>
       </c>
       <c r="V5" t="n">
-        <v>0.4631254699260249</v>
+        <v>0.9290759899563976</v>
       </c>
       <c r="W5" t="n">
-        <v>0.4818863289892688</v>
+        <v>0.6243283866723438</v>
       </c>
       <c r="X5" t="n">
-        <v>0.4620181227538789</v>
+        <v>0.5409737059831639</v>
       </c>
     </row>
     <row r="6">
@@ -868,7 +868,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>dit</t>
+          <t>flowbot</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -880,64 +880,64 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2444131834987684</v>
+        <v>0.7138278559596645</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2142518646851799</v>
+        <v>0.9289711072750856</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2999593995204876</v>
+        <v>0.9514460108732092</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4704990818499143</v>
+        <v>0.9518634328757024</v>
       </c>
       <c r="I6" t="n">
-        <v>0.4996864740313642</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>0.4672847098895506</v>
+        <v>0.9370209920996716</v>
       </c>
       <c r="K6" t="n">
-        <v>0.4702345911003359</v>
+        <v>0.9242445997784808</v>
       </c>
       <c r="L6" t="n">
-        <v>0.4245115289026513</v>
+        <v>0.8589363510185869</v>
       </c>
       <c r="M6" t="n">
-        <v>0.2292962878846571</v>
+        <v>0.3082338336756623</v>
       </c>
       <c r="N6" t="n">
-        <v>0.465953801595318</v>
+        <v>0.933658158614168</v>
       </c>
       <c r="O6" t="n">
-        <v>0.4522589791969921</v>
+        <v>0.9514086154617384</v>
       </c>
       <c r="P6" t="n">
-        <v>0.4360517684341455</v>
+        <v>0.8948717248922784</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.3763252173277657</v>
+        <v>0.8518262214254619</v>
       </c>
       <c r="R6" t="n">
-        <v>0.4277534948164282</v>
+        <v>0.9263976798275305</v>
       </c>
       <c r="S6" t="n">
-        <v>0.2351334954311624</v>
+        <v>0.9149756229122948</v>
       </c>
       <c r="T6" t="n">
-        <v>0.1040047387135331</v>
+        <v>0.9257741993657416</v>
       </c>
       <c r="U6" t="n">
-        <v>0.3148453397298317</v>
+        <v>0.3157468635106495</v>
       </c>
       <c r="V6" t="n">
-        <v>0.4702996682168844</v>
+        <v>0.9262509398520498</v>
       </c>
       <c r="W6" t="n">
-        <v>0.3742207483963599</v>
+        <v>0.9637726579785376</v>
       </c>
       <c r="X6" t="n">
-        <v>0.4592801200341593</v>
+        <v>0.9240362455077578</v>
       </c>
     </row>
     <row r="7">
@@ -946,7 +946,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>pndit</t>
+          <t>dit</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -958,64 +958,64 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3314563098857423</v>
+        <v>0.4888263669975369</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3733300491210188</v>
+        <v>0.4285037293703598</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4449691623235021</v>
+        <v>0.5999187990409752</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3707845573949172</v>
+        <v>0.9409981636998286</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5</v>
+        <v>0.9993729480627284</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4743599780183689</v>
+        <v>0.9345694197791012</v>
       </c>
       <c r="K7" t="n">
-        <v>0.4554416071219631</v>
+        <v>0.9404691822006718</v>
       </c>
       <c r="L7" t="n">
-        <v>0.4444828077577407</v>
+        <v>0.8490230578053026</v>
       </c>
       <c r="M7" t="n">
-        <v>0.6301270315450321</v>
+        <v>0.3057283838462095</v>
       </c>
       <c r="N7" t="n">
-        <v>0.4162722804238599</v>
+        <v>0.931907603190636</v>
       </c>
       <c r="O7" t="n">
-        <v>0.4572410903774924</v>
+        <v>0.9045179583939842</v>
       </c>
       <c r="P7" t="n">
-        <v>0.4426851123661015</v>
+        <v>0.8692535253098979</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.4522442199582824</v>
+        <v>0.7526504346555315</v>
       </c>
       <c r="R7" t="n">
-        <v>0.4221994527856645</v>
+        <v>0.8555069896328563</v>
       </c>
       <c r="S7" t="n">
-        <v>0.2985081524520012</v>
+        <v>0.4702669908623247</v>
       </c>
       <c r="T7" t="n">
-        <v>0.3253560488821521</v>
+        <v>0.2080094774270662</v>
       </c>
       <c r="U7" t="n">
-        <v>0.1672064938119258</v>
+        <v>0.6296906794596634</v>
       </c>
       <c r="V7" t="n">
-        <v>0.469362492404946</v>
+        <v>0.9405993364337688</v>
       </c>
       <c r="W7" t="n">
-        <v>0.4801381965459451</v>
+        <v>0.7484414967927199</v>
       </c>
       <c r="X7" t="n">
-        <v>0.4666021481992194</v>
+        <v>0.9185602400683186</v>
       </c>
     </row>
     <row r="8">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>hisdit</t>
+          <t>pndit</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1036,64 +1036,64 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3654243236157181</v>
+        <v>0.6629126197714845</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2561263504879341</v>
+        <v>0.7466600982420376</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4123824429857261</v>
+        <v>0.8899383246470043</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4653716012437186</v>
+        <v>0.7415691147898343</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>0.4712459829739629</v>
+        <v>0.9487199560367378</v>
       </c>
       <c r="K8" t="n">
-        <v>0.4769648420638276</v>
+        <v>0.9108832142439263</v>
       </c>
       <c r="L8" t="n">
-        <v>0.3</v>
+        <v>0.8889656155154814</v>
       </c>
       <c r="M8" t="n">
-        <v>0.7232028580043454</v>
+        <v>0.8401693753933762</v>
       </c>
       <c r="N8" t="n">
-        <v>0.4656993727782814</v>
+        <v>0.8325445608477199</v>
       </c>
       <c r="O8" t="n">
-        <v>0.4548433756634232</v>
+        <v>0.9144821807549848</v>
       </c>
       <c r="P8" t="n">
-        <v>0.4620936217945651</v>
+        <v>0.8824768579847121</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.4109776164407308</v>
+        <v>0.9044884399165648</v>
       </c>
       <c r="R8" t="n">
-        <v>0.3875922347430473</v>
+        <v>0.844398905571329</v>
       </c>
       <c r="S8" t="n">
-        <v>0.465586641436309</v>
+        <v>0.5970163049040024</v>
       </c>
       <c r="T8" t="n">
-        <v>0.3807234964526264</v>
+        <v>0.6507120977643042</v>
       </c>
       <c r="U8" t="n">
-        <v>0.3158433710366288</v>
+        <v>0.3344129876238517</v>
       </c>
       <c r="V8" t="n">
-        <v>0.4715265700482382</v>
+        <v>0.938724984809892</v>
       </c>
       <c r="W8" t="n">
-        <v>0.4188700455853451</v>
+        <v>0.9602763930918902</v>
       </c>
       <c r="X8" t="n">
-        <v>0.4654356901072616</v>
+        <v>0.9332042963984388</v>
       </c>
     </row>
     <row r="9">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>pnhisdit</t>
+          <t>hisdit</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1114,132 +1114,288 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.7186300891539206</v>
+        <v>0.7308486472314362</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5131158511546914</v>
+        <v>0.5122527009758682</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8750822854995077</v>
+        <v>0.8247648859714521</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8524894037806426</v>
+        <v>0.9307432024874372</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9997764379132299</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.9515411455930542</v>
+        <v>0.9424919659479258</v>
       </c>
       <c r="K9" t="n">
-        <v>0.9439377880729315</v>
+        <v>0.9539296841276552</v>
       </c>
       <c r="L9" t="n">
-        <v>0.7039948280943551</v>
+        <v>0.6</v>
       </c>
       <c r="M9" t="n">
-        <v>0.955847438786497</v>
+        <v>0.9642704773391272</v>
       </c>
       <c r="N9" t="n">
-        <v>0.9343810399839774</v>
+        <v>0.9313987455565628</v>
       </c>
       <c r="O9" t="n">
-        <v>0.9364383391315788</v>
+        <v>0.9096867513268464</v>
       </c>
       <c r="P9" t="n">
-        <v>0.9300766722048101</v>
+        <v>0.921167023838839</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.8805039452864243</v>
+        <v>0.8219552328814616</v>
       </c>
       <c r="R9" t="n">
-        <v>0.8608260001250898</v>
+        <v>0.7751844694860945</v>
       </c>
       <c r="S9" t="n">
-        <v>0.9330233351219714</v>
+        <v>0.931173282872618</v>
       </c>
       <c r="T9" t="n">
-        <v>0.8291675597854449</v>
+        <v>0.7614469929052529</v>
       </c>
       <c r="U9" t="n">
-        <v>0.7247415268509968</v>
+        <v>0.6316867420732576</v>
       </c>
       <c r="V9" t="n">
-        <v>0.9395545270803949</v>
+        <v>0.9430531400964764</v>
       </c>
       <c r="W9" t="n">
-        <v>0.845763941273068</v>
+        <v>0.8377400911706901</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9318727292525838</v>
+        <v>0.9308713802145232</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>pnhisdit</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>sgp</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
       <c r="E10" t="n">
+        <v>0.7064115310764051</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.5139790013335145</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9253996850275632</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.774235605073848</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.9995528758264598</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.9605903252381828</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.9339458920182081</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.8079896561887102</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.3101927743762022</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.937363334411392</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.9631899269363112</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.9329073880727108</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.939052657691387</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.946467530764085</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.934873387371325</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.8968881266656368</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.817796311628736</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.9360559140643132</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.8537877913754456</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.9328740782906444</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>hisditonly</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>sgp</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.961556856628588</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0889405835347683</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.2613828534507007</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.9410201566134628</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.9396101939917234</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.9589084133678036</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.6350873887600679</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.7902257641030861</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.932266467500007</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.8928541108167063</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.9037870681214863</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.9082900596185676</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.9229921306942644</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.0226352728866066</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.3537579683589634</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.93770971462465</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.6502681884210223</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.5771985225235223</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4</v>
+      </c>
+      <c r="H12" t="n">
+        <v>11</v>
+      </c>
+      <c r="I12" t="n">
+        <v>5</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" t="n">
+        <v>11</v>
+      </c>
+      <c r="L12" t="n">
+        <v>5</v>
+      </c>
+      <c r="M12" t="n">
+        <v>3</v>
+      </c>
+      <c r="N12" t="n">
+        <v>15</v>
+      </c>
+      <c r="O12" t="n">
+        <v>49</v>
+      </c>
+      <c r="P12" t="n">
+        <v>153</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>9</v>
+      </c>
+      <c r="R12" t="n">
+        <v>5</v>
+      </c>
+      <c r="S12" t="n">
+        <v>3</v>
+      </c>
+      <c r="T12" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" t="n">
+        <v>3</v>
+      </c>
+      <c r="V12" t="n">
         <v>8</v>
       </c>
-      <c r="F10" t="n">
+      <c r="W12" t="n">
+        <v>7</v>
+      </c>
+      <c r="X12" t="n">
         <v>4</v>
-      </c>
-      <c r="G10" t="n">
-        <v>8</v>
-      </c>
-      <c r="H10" t="n">
-        <v>22</v>
-      </c>
-      <c r="I10" t="n">
-        <v>10</v>
-      </c>
-      <c r="J10" t="n">
-        <v>4</v>
-      </c>
-      <c r="K10" t="n">
-        <v>22</v>
-      </c>
-      <c r="L10" t="n">
-        <v>10</v>
-      </c>
-      <c r="M10" t="n">
-        <v>4</v>
-      </c>
-      <c r="N10" t="n">
-        <v>30</v>
-      </c>
-      <c r="O10" t="n">
-        <v>98</v>
-      </c>
-      <c r="P10" t="n">
-        <v>305</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>18</v>
-      </c>
-      <c r="R10" t="n">
-        <v>10</v>
-      </c>
-      <c r="S10" t="n">
-        <v>6</v>
-      </c>
-      <c r="T10" t="n">
-        <v>2</v>
-      </c>
-      <c r="U10" t="n">
-        <v>6</v>
-      </c>
-      <c r="V10" t="n">
-        <v>16</v>
-      </c>
-      <c r="W10" t="n">
-        <v>14</v>
-      </c>
-      <c r="X10" t="n">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hipndit, analysis, codes for real robot
</commit_message>
<xml_diff>
--- a/notebooks/simulation/sim_results/summary_norm_dist_000_test.xlsx
+++ b/notebooks/simulation/sim_results/summary_norm_dist_000_test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -946,76 +946,76 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>flowbot</t>
+          <t>flowbotallopen</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>sgp</t>
+          <t>raw</t>
         </is>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7138278559596645</v>
+        <v>0.5775957040770099</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9289711072750856</v>
+        <v>0.5872966996688901</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9514460108732092</v>
+        <v>0.9435511942718612</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9518634328757024</v>
+        <v>0.726889918262501</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9370209920996716</v>
+        <v>0.4581593895024392</v>
       </c>
       <c r="K7" t="n">
-        <v>0.9242445997784808</v>
+        <v>0.8674649961167815</v>
       </c>
       <c r="L7" t="n">
-        <v>0.8589363510185869</v>
+        <v>0.8420231239051486</v>
       </c>
       <c r="M7" t="n">
-        <v>0.3082338336756623</v>
+        <v>0.02006576500047157</v>
       </c>
       <c r="N7" t="n">
-        <v>0.933658158614168</v>
+        <v>0.6414610853430778</v>
       </c>
       <c r="O7" t="n">
-        <v>0.9514086154617384</v>
+        <v>0.8644771565725876</v>
       </c>
       <c r="P7" t="n">
-        <v>0.8948717248922784</v>
+        <v>0.7747019942539959</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.8518262214254619</v>
+        <v>0.7308324085738898</v>
       </c>
       <c r="R7" t="n">
-        <v>0.9263976798275305</v>
+        <v>0.7975350667878882</v>
       </c>
       <c r="S7" t="n">
-        <v>0.9149756229122948</v>
+        <v>0.9218991476965369</v>
       </c>
       <c r="T7" t="n">
-        <v>0.9257741993657416</v>
+        <v>0.0002909031672504</v>
       </c>
       <c r="U7" t="n">
-        <v>0.3157468635106495</v>
+        <v>0.5747286531041927</v>
       </c>
       <c r="V7" t="n">
-        <v>0.9262509398520498</v>
+        <v>0.921810695179186</v>
       </c>
       <c r="W7" t="n">
-        <v>0.9637726579785376</v>
+        <v>0.8962025627950905</v>
       </c>
       <c r="X7" t="n">
-        <v>0.9240362455077578</v>
+        <v>0.90144058608341</v>
       </c>
     </row>
     <row r="8">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>dit</t>
+          <t>flowbot</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1036,64 +1036,64 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4888263669975369</v>
+        <v>0.7138278559596645</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4285037293703598</v>
+        <v>0.9289711072750856</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5999187990409752</v>
+        <v>0.9514460108732092</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9409981636998286</v>
+        <v>0.9518634328757024</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9993729480627284</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>0.9345694197791012</v>
+        <v>0.9370209920996716</v>
       </c>
       <c r="K8" t="n">
-        <v>0.9404691822006718</v>
+        <v>0.9242445997784808</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8490230578053026</v>
+        <v>0.8589363510185869</v>
       </c>
       <c r="M8" t="n">
-        <v>0.3057283838462095</v>
+        <v>0.3082338336756623</v>
       </c>
       <c r="N8" t="n">
-        <v>0.931907603190636</v>
+        <v>0.933658158614168</v>
       </c>
       <c r="O8" t="n">
-        <v>0.9045179583939842</v>
+        <v>0.9514086154617384</v>
       </c>
       <c r="P8" t="n">
-        <v>0.8692535253098979</v>
+        <v>0.8948717248922784</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.7526504346555315</v>
+        <v>0.8518262214254619</v>
       </c>
       <c r="R8" t="n">
-        <v>0.8555069896328563</v>
+        <v>0.9263976798275305</v>
       </c>
       <c r="S8" t="n">
-        <v>0.4702669908623247</v>
+        <v>0.9149756229122948</v>
       </c>
       <c r="T8" t="n">
-        <v>0.2080094774270662</v>
+        <v>0.9257741993657416</v>
       </c>
       <c r="U8" t="n">
-        <v>0.6296906794596634</v>
+        <v>0.3157468635106495</v>
       </c>
       <c r="V8" t="n">
-        <v>0.9405993364337688</v>
+        <v>0.9262509398520498</v>
       </c>
       <c r="W8" t="n">
-        <v>0.7484414967927199</v>
+        <v>0.9637726579785376</v>
       </c>
       <c r="X8" t="n">
-        <v>0.9185602400683186</v>
+        <v>0.9240362455077578</v>
       </c>
     </row>
     <row r="9">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>pndit</t>
+          <t>dit</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1114,64 +1114,64 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6629126197714845</v>
+        <v>0.4888263669975369</v>
       </c>
       <c r="F9" t="n">
-        <v>0.7466600982420376</v>
+        <v>0.4285037293703598</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8899383246470043</v>
+        <v>0.5999187990409752</v>
       </c>
       <c r="H9" t="n">
-        <v>0.7415691147898343</v>
+        <v>0.9409981636998286</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0.9993729480627284</v>
       </c>
       <c r="J9" t="n">
-        <v>0.9487199560367378</v>
+        <v>0.9345694197791012</v>
       </c>
       <c r="K9" t="n">
-        <v>0.9108832142439263</v>
+        <v>0.9404691822006718</v>
       </c>
       <c r="L9" t="n">
-        <v>0.8889656155154814</v>
+        <v>0.8490230578053026</v>
       </c>
       <c r="M9" t="n">
-        <v>0.8401693753933762</v>
+        <v>0.3057283838462095</v>
       </c>
       <c r="N9" t="n">
-        <v>0.8325445608477199</v>
+        <v>0.931907603190636</v>
       </c>
       <c r="O9" t="n">
-        <v>0.9144821807549848</v>
+        <v>0.9045179583939842</v>
       </c>
       <c r="P9" t="n">
-        <v>0.8824768579847121</v>
+        <v>0.8692535253098979</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.9044884399165648</v>
+        <v>0.7526504346555315</v>
       </c>
       <c r="R9" t="n">
-        <v>0.844398905571329</v>
+        <v>0.8555069896328563</v>
       </c>
       <c r="S9" t="n">
-        <v>0.5970163049040024</v>
+        <v>0.4702669908623247</v>
       </c>
       <c r="T9" t="n">
-        <v>0.6507120977643042</v>
+        <v>0.2080094774270662</v>
       </c>
       <c r="U9" t="n">
-        <v>0.3344129876238517</v>
+        <v>0.6296906794596634</v>
       </c>
       <c r="V9" t="n">
-        <v>0.938724984809892</v>
+        <v>0.9405993364337688</v>
       </c>
       <c r="W9" t="n">
-        <v>0.9602763930918902</v>
+        <v>0.7484414967927199</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9332042963984388</v>
+        <v>0.9185602400683186</v>
       </c>
     </row>
     <row r="10">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>hisdit</t>
+          <t>pndit</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1192,64 +1192,64 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7308486472314362</v>
+        <v>0.6629126197714845</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5122527009758682</v>
+        <v>0.7466600982420376</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8247648859714521</v>
+        <v>0.8899383246470043</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9307432024874372</v>
+        <v>0.7415691147898343</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0.9424919659479258</v>
+        <v>0.9487199560367378</v>
       </c>
       <c r="K10" t="n">
-        <v>0.9539296841276552</v>
+        <v>0.9108832142439263</v>
       </c>
       <c r="L10" t="n">
-        <v>0.6</v>
+        <v>0.8889656155154814</v>
       </c>
       <c r="M10" t="n">
-        <v>0.9642704773391272</v>
+        <v>0.8401693753933762</v>
       </c>
       <c r="N10" t="n">
-        <v>0.9313987455565628</v>
+        <v>0.8325445608477199</v>
       </c>
       <c r="O10" t="n">
-        <v>0.9096867513268464</v>
+        <v>0.9144821807549848</v>
       </c>
       <c r="P10" t="n">
-        <v>0.921167023838839</v>
+        <v>0.8824768579847121</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.8219552328814616</v>
+        <v>0.9044884399165648</v>
       </c>
       <c r="R10" t="n">
-        <v>0.7751844694860945</v>
+        <v>0.844398905571329</v>
       </c>
       <c r="S10" t="n">
-        <v>0.931173282872618</v>
+        <v>0.5970163049040024</v>
       </c>
       <c r="T10" t="n">
-        <v>0.7614469929052529</v>
+        <v>0.6507120977643042</v>
       </c>
       <c r="U10" t="n">
-        <v>0.6316867420732576</v>
+        <v>0.3344129876238517</v>
       </c>
       <c r="V10" t="n">
-        <v>0.9430531400964764</v>
+        <v>0.938724984809892</v>
       </c>
       <c r="W10" t="n">
-        <v>0.8377400911706901</v>
+        <v>0.9602763930918902</v>
       </c>
       <c r="X10" t="n">
-        <v>0.9308713802145232</v>
+        <v>0.9332042963984388</v>
       </c>
     </row>
     <row r="11">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>pnhisdit</t>
+          <t>hisdit</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1270,64 +1270,64 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7064115310764051</v>
+        <v>0.7308486472314362</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5139790013335145</v>
+        <v>0.5122527009758682</v>
       </c>
       <c r="G11" t="n">
-        <v>0.9253996850275632</v>
+        <v>0.8247648859714521</v>
       </c>
       <c r="H11" t="n">
-        <v>0.774235605073848</v>
+        <v>0.9307432024874372</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9995528758264598</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>0.9605903252381828</v>
+        <v>0.9424919659479258</v>
       </c>
       <c r="K11" t="n">
-        <v>0.9339458920182081</v>
+        <v>0.9539296841276552</v>
       </c>
       <c r="L11" t="n">
-        <v>0.8079896561887102</v>
+        <v>0.6</v>
       </c>
       <c r="M11" t="n">
-        <v>0.3101927743762022</v>
+        <v>0.9642704773391272</v>
       </c>
       <c r="N11" t="n">
-        <v>0.937363334411392</v>
+        <v>0.9313987455565628</v>
       </c>
       <c r="O11" t="n">
-        <v>0.9631899269363112</v>
+        <v>0.9096867513268464</v>
       </c>
       <c r="P11" t="n">
-        <v>0.9329073880727108</v>
+        <v>0.921167023838839</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.939052657691387</v>
+        <v>0.8219552328814616</v>
       </c>
       <c r="R11" t="n">
-        <v>0.946467530764085</v>
+        <v>0.7751844694860945</v>
       </c>
       <c r="S11" t="n">
-        <v>0.934873387371325</v>
+        <v>0.931173282872618</v>
       </c>
       <c r="T11" t="n">
-        <v>0.8968881266656368</v>
+        <v>0.7614469929052529</v>
       </c>
       <c r="U11" t="n">
-        <v>0.817796311628736</v>
+        <v>0.6316867420732576</v>
       </c>
       <c r="V11" t="n">
-        <v>0.9360559140643132</v>
+        <v>0.9430531400964764</v>
       </c>
       <c r="W11" t="n">
-        <v>0.8537877913754456</v>
+        <v>0.8377400911706901</v>
       </c>
       <c r="X11" t="n">
-        <v>0.9328740782906444</v>
+        <v>0.9308713802145232</v>
       </c>
     </row>
     <row r="12">
@@ -1336,7 +1336,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>hisditonly</t>
+          <t>pnhisdit</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1348,64 +1348,64 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.961556856628588</v>
+        <v>0.7064115310764051</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0889405835347683</v>
+        <v>0.5139790013335145</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2613828534507007</v>
+        <v>0.9253996850275632</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9410201566134628</v>
+        <v>0.774235605073848</v>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0.9995528758264598</v>
       </c>
       <c r="J12" t="n">
-        <v>0.9396101939917234</v>
+        <v>0.9605903252381828</v>
       </c>
       <c r="K12" t="n">
-        <v>0.9589084133678036</v>
+        <v>0.9339458920182081</v>
       </c>
       <c r="L12" t="n">
-        <v>0.8</v>
+        <v>0.8079896561887102</v>
       </c>
       <c r="M12" t="n">
-        <v>0.6350873887600679</v>
+        <v>0.3101927743762022</v>
       </c>
       <c r="N12" t="n">
-        <v>0.7902257641030861</v>
+        <v>0.937363334411392</v>
       </c>
       <c r="O12" t="n">
-        <v>0.932266467500007</v>
+        <v>0.9631899269363112</v>
       </c>
       <c r="P12" t="n">
-        <v>0.8928541108167063</v>
+        <v>0.9329073880727108</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.9037870681214863</v>
+        <v>0.939052657691387</v>
       </c>
       <c r="R12" t="n">
-        <v>0.9082900596185676</v>
+        <v>0.946467530764085</v>
       </c>
       <c r="S12" t="n">
-        <v>0.9229921306942644</v>
+        <v>0.934873387371325</v>
       </c>
       <c r="T12" t="n">
-        <v>0.0226352728866066</v>
+        <v>0.8968881266656368</v>
       </c>
       <c r="U12" t="n">
-        <v>0.3537579683589634</v>
+        <v>0.817796311628736</v>
       </c>
       <c r="V12" t="n">
-        <v>0.93770971462465</v>
+        <v>0.9360559140643132</v>
       </c>
       <c r="W12" t="n">
-        <v>0.6502681884210223</v>
+        <v>0.8537877913754456</v>
       </c>
       <c r="X12" t="n">
-        <v>0.5771985225235223</v>
+        <v>0.9328740782906444</v>
       </c>
     </row>
     <row r="13">
@@ -1414,7 +1414,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>hisonly</t>
+          <t>hisditonly</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1426,64 +1426,64 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5544635472149846</v>
+        <v>0.961556856628588</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2169871603250254</v>
+        <v>0.0889405835347683</v>
       </c>
       <c r="G13" t="n">
-        <v>0.25</v>
+        <v>0.2613828534507007</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9589802279644588</v>
+        <v>0.9410201566134628</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>0.4747361688593852</v>
+        <v>0.9396101939917234</v>
       </c>
       <c r="K13" t="n">
-        <v>0.9484331168438956</v>
+        <v>0.9589084133678036</v>
       </c>
       <c r="L13" t="n">
         <v>0.8</v>
       </c>
       <c r="M13" t="n">
-        <v>0.02981696275251493</v>
+        <v>0.6350873887600679</v>
       </c>
       <c r="N13" t="n">
-        <v>0.7582339347824775</v>
+        <v>0.7902257641030861</v>
       </c>
       <c r="O13" t="n">
-        <v>0.9211910785569832</v>
+        <v>0.932266467500007</v>
       </c>
       <c r="P13" t="n">
-        <v>0.8453338233183735</v>
+        <v>0.8928541108167063</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.7943689685785805</v>
+        <v>0.9037870681214863</v>
       </c>
       <c r="R13" t="n">
-        <v>0.7508333214522451</v>
+        <v>0.9082900596185676</v>
       </c>
       <c r="S13" t="n">
-        <v>0.8102698814761254</v>
+        <v>0.9229921306942644</v>
       </c>
       <c r="T13" t="n">
-        <v>0.0118553015307967</v>
+        <v>0.0226352728866066</v>
       </c>
       <c r="U13" t="n">
-        <v>0.3062005729272828</v>
+        <v>0.3537579683589634</v>
       </c>
       <c r="V13" t="n">
-        <v>0.8153569488872587</v>
+        <v>0.93770971462465</v>
       </c>
       <c r="W13" t="n">
-        <v>0.6746233693233445</v>
+        <v>0.6502681884210223</v>
       </c>
       <c r="X13" t="n">
-        <v>0.800184658812862</v>
+        <v>0.5771985225235223</v>
       </c>
     </row>
     <row r="14">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>hispndit01only1</t>
+          <t>hisonly</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1504,64 +1504,64 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.4998536620899018</v>
+        <v>0.5544635472149846</v>
       </c>
       <c r="F14" t="n">
-        <v>0.4600816414688248</v>
+        <v>0.2169871603250254</v>
       </c>
       <c r="G14" t="n">
-        <v>0.7042326608511079</v>
+        <v>0.25</v>
       </c>
       <c r="H14" t="n">
-        <v>0.8556819656035262</v>
+        <v>0.9589802279644588</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>0.06326970381719681</v>
+        <v>0.4747361688593852</v>
       </c>
       <c r="K14" t="n">
-        <v>0.9462492887723564</v>
+        <v>0.9484331168438956</v>
       </c>
       <c r="L14" t="n">
         <v>0.8</v>
       </c>
       <c r="M14" t="n">
-        <v>0.1501407124505755</v>
+        <v>0.02981696275251493</v>
       </c>
       <c r="N14" t="n">
-        <v>0.9254747642868872</v>
+        <v>0.7582339347824775</v>
       </c>
       <c r="O14" t="n">
-        <v>0.65425785997176</v>
+        <v>0.9211910785569832</v>
       </c>
       <c r="P14" t="n">
-        <v>0.8485297706378859</v>
+        <v>0.8453338233183735</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.6083053807963705</v>
+        <v>0.7943689685785805</v>
       </c>
       <c r="R14" t="n">
-        <v>0.94960823950261</v>
+        <v>0.7508333214522451</v>
       </c>
       <c r="S14" t="n">
-        <v>0.9268528052811966</v>
+        <v>0.8102698814761254</v>
       </c>
       <c r="T14" t="n">
-        <v>0.0180879897693859</v>
+        <v>0.0118553015307967</v>
       </c>
       <c r="U14" t="n">
-        <v>0.3914028262774722</v>
+        <v>0.3062005729272828</v>
       </c>
       <c r="V14" t="n">
-        <v>0.9309674603013888</v>
+        <v>0.8153569488872587</v>
       </c>
       <c r="W14" t="n">
-        <v>0.8401280888065562</v>
+        <v>0.6746233693233445</v>
       </c>
       <c r="X14" t="n">
-        <v>0.923391224989434</v>
+        <v>0.800184658812862</v>
       </c>
     </row>
     <row r="15">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>hispndit01only2</t>
+          <t>pndit&amp;pn++</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1582,131 +1582,599 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2437702523372877</v>
+        <v>0.4691307207856198</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4756847969034869</v>
+        <v>0.9400283511907082</v>
       </c>
       <c r="G15" t="n">
-        <v>0.9385602898594668</v>
+        <v>0.7322693818116437</v>
       </c>
       <c r="H15" t="n">
-        <v>0.9583419139390944</v>
+        <v>0.8508917738562736</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>0.922363107890853</v>
+        <v>0.925228467493984</v>
       </c>
       <c r="K15" t="n">
-        <v>0.9652186422818499</v>
+        <v>0.956889624458642</v>
       </c>
       <c r="L15" t="n">
-        <v>0.8500137886018606</v>
+        <v>0.8900924665670253</v>
       </c>
       <c r="M15" t="n">
-        <v>0.141654922463736</v>
+        <v>0.3063550206833829</v>
       </c>
       <c r="N15" t="n">
-        <v>0.9062325676218984</v>
+        <v>0.9348710260721662</v>
       </c>
       <c r="O15" t="n">
-        <v>0.8405068098278329</v>
+        <v>0.9363529922657632</v>
       </c>
       <c r="P15" t="n">
-        <v>0.88834776681867</v>
+        <v>0.914531368814017</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.7293376994864654</v>
+        <v>0.9276253228939298</v>
       </c>
       <c r="R15" t="n">
-        <v>0.9377039098311106</v>
+        <v>0.932984219744539</v>
       </c>
       <c r="S15" t="n">
-        <v>0.9377426842601526</v>
+        <v>0.9449465116806404</v>
       </c>
       <c r="T15" t="n">
-        <v>0.9108828266632898</v>
+        <v>0.9206073802550248</v>
       </c>
       <c r="U15" t="n">
-        <v>0.6325450934627354</v>
+        <v>0.3584884745848697</v>
       </c>
       <c r="V15" t="n">
-        <v>0.9286577108090888</v>
+        <v>0.9354923638755008</v>
       </c>
       <c r="W15" t="n">
-        <v>0.8547147935632159</v>
+        <v>0.8717896628163613</v>
       </c>
       <c r="X15" t="n">
-        <v>0.9110975858697772</v>
+        <v>0.9346662340419836</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>dit&amp;pn++</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>sgp</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
       <c r="E16" t="n">
+        <v>0.7301867218910854</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9317058211891958</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.8627579999030595</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.9479817257937072</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.918611770065529</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.9771820886466894</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.8377455714585403</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.3129463861646694</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.934907087247616</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.9179893990231394</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.9093645087721356</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.8243519357848043</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.9428792186473928</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.9293936465152882</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.9228225167519656</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.3584748582902033</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.929701927956842</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.8753540034520791</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0.9106394042777139</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>largedit&amp;pn++</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sgp</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.7273269810970115</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.8995981881489632</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.7109559285660698</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.9395127144785804</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.9515306872093762</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.927219227743634</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.8449673620617937</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.3053521311551217</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.9268652402953752</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.8053098102033086</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.9034545771158181</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.7229976504790084</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.7579144059760083</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.9415611758402678</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.8875957653621757</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.956898775000406</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.9301295195484586</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.8866346314810067</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0.9329968447669564</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>flowbotallopen</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sgp</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.6810513221671851</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.6417785242810977</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.9273562855000586</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.9576042138624502</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.7807644094262043</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.8711505701242831</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.8434000822207519</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.79928164814905</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.9544092831270539</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.8959796651393381</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.8360227341682046</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.9572299156137444</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.9303038269138458</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.0149991764431838</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.3853901168825424</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.923231732317806</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0.8475350762788363</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0.8574471090636353</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>pndit&amp;pn++allopen&gt;005</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>sgp</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.6296061724169432</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.922255040912476</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.9390989833054656</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.9676421289570594</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.950465941929064</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.9222544849126231</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.837403060953738</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.4368373423512981</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.9338466924047708</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.9054860799661724</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.943067027671105</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.9389742083057596</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.7586843838535584</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.6313566429005669</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.921188757063587</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.3814672994790609</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0.9396433026330286</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0.8677833542640851</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0.9404987523568654</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>dit&amp;pn++allopen&gt;01</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>sgp</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.7189512005241321</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.9485654653040948</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.7041576718646176</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.8503720907971369</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.9449888747185105</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.9125739998881752</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.6423432299286097</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.3099760283648656</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.7899385039863834</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.8609342291449414</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.8887371525787127</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.8352117209873667</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.756063711584696</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.6333896704647582</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.9317831109813114</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.6464667381068901</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0.9373351108470954</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0.8268744124933202</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0.6941901958087614</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>hispnditckpt299</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>sgp</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.6383061445139828</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.4859589221426986</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.8309260976759134</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.9559541569516719</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.9748837861596176</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.9389391153707609</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.8933586607942084</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.1934708289242569</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.937902792284849</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.9485533316394013</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.9208433663887449</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.9187426819475297</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.7213693535465666</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.8691632039796019</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.9313143224087592</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0.314294727323924</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0.9242476046829284</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0.9025091162043726</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0.9121223877874056</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="n">
         <v>4</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F22" t="n">
         <v>2</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G22" t="n">
         <v>4</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H22" t="n">
         <v>11</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I22" t="n">
         <v>5</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J22" t="n">
         <v>2</v>
       </c>
-      <c r="K16" t="n">
+      <c r="K22" t="n">
         <v>11</v>
       </c>
-      <c r="L16" t="n">
+      <c r="L22" t="n">
         <v>5</v>
       </c>
-      <c r="M16" t="n">
+      <c r="M22" t="n">
         <v>3</v>
       </c>
-      <c r="N16" t="n">
+      <c r="N22" t="n">
         <v>15</v>
       </c>
-      <c r="O16" t="n">
+      <c r="O22" t="n">
         <v>49</v>
       </c>
-      <c r="P16" t="n">
+      <c r="P22" t="n">
         <v>153</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="Q22" t="n">
         <v>9</v>
       </c>
-      <c r="R16" t="n">
+      <c r="R22" t="n">
         <v>5</v>
       </c>
-      <c r="S16" t="n">
+      <c r="S22" t="n">
         <v>3</v>
       </c>
-      <c r="T16" t="n">
+      <c r="T22" t="n">
         <v>1</v>
       </c>
-      <c r="U16" t="n">
+      <c r="U22" t="n">
         <v>3</v>
       </c>
-      <c r="V16" t="n">
+      <c r="V22" t="n">
         <v>8</v>
       </c>
-      <c r="W16" t="n">
+      <c r="W22" t="n">
         <v>7</v>
       </c>
-      <c r="X16" t="n">
+      <c r="X22" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add filter in simulation
</commit_message>
<xml_diff>
--- a/notebooks/simulation/sim_results/summary_norm_dist_000_test.xlsx
+++ b/notebooks/simulation/sim_results/summary_norm_dist_000_test.xlsx
@@ -2038,7 +2038,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>hispnditckpt299</t>
+          <t>hispnditFilter</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2050,64 +2050,64 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.6383061445139828</v>
+        <v>0.7010818321629645</v>
       </c>
       <c r="F21" t="n">
-        <v>0.4859589221426986</v>
+        <v>0.7594578184086344</v>
       </c>
       <c r="G21" t="n">
-        <v>0.8309260976759134</v>
+        <v>0.9456563717395856</v>
       </c>
       <c r="H21" t="n">
-        <v>0.9559541569516719</v>
+        <v>0.9519998607969392</v>
       </c>
       <c r="I21" t="n">
         <v>1</v>
       </c>
       <c r="J21" t="n">
-        <v>0.9748837861596176</v>
+        <v>0.6773292179153978</v>
       </c>
       <c r="K21" t="n">
-        <v>0.9389391153707609</v>
+        <v>0.9466433269072861</v>
       </c>
       <c r="L21" t="n">
-        <v>0.8933586607942084</v>
+        <v>0.8467233258443898</v>
       </c>
       <c r="M21" t="n">
-        <v>0.1934708289242569</v>
+        <v>0.3099058898395918</v>
       </c>
       <c r="N21" t="n">
-        <v>0.937902792284849</v>
+        <v>0.9273430168101348</v>
       </c>
       <c r="O21" t="n">
-        <v>0.9485533316394013</v>
+        <v>0.9666784585856899</v>
       </c>
       <c r="P21" t="n">
-        <v>0.9208433663887449</v>
+        <v>0.944557729599292</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.9187426819475297</v>
+        <v>0.8718373137109566</v>
       </c>
       <c r="R21" t="n">
-        <v>0.7213693535465666</v>
+        <v>0.940175527682934</v>
       </c>
       <c r="S21" t="n">
-        <v>0.8691632039796019</v>
+        <v>0.943025451569925</v>
       </c>
       <c r="T21" t="n">
-        <v>0.9313143224087592</v>
+        <v>0.9052271878411812</v>
       </c>
       <c r="U21" t="n">
-        <v>0.314294727323924</v>
+        <v>0.3556506702809143</v>
       </c>
       <c r="V21" t="n">
-        <v>0.9242476046829284</v>
+        <v>0.9359142068168036</v>
       </c>
       <c r="W21" t="n">
-        <v>0.9025091162043726</v>
+        <v>0.9131209728303235</v>
       </c>
       <c r="X21" t="n">
-        <v>0.9121223877874056</v>
+        <v>0.9400022208139552</v>
       </c>
     </row>
     <row r="22">

</xml_diff>